<commit_message>
[wa_dnr_forest_health_tracker/#1456] Add/edit project grants (child) - Updating Region table to include RegionAbbrev. Adding RegionID to GrantAllocation.
</commit_message>
<xml_diff>
--- a/Database/SourceExcelFiles/FuzzyMatchingOut.xlsx
+++ b/Database/SourceExcelFiles/FuzzyMatchingOut.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\wadnrforesthealth\Database\SourceExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EA23EA-1CD9-46B3-B1C6-2A732EC0D640}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="28365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="90">
   <si>
     <t>REGION</t>
   </si>
@@ -290,23 +295,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -321,26 +327,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -628,20 +651,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,8 +680,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -668,12 +693,12 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -685,12 +710,12 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -702,12 +727,12 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.9803921568627451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="n">
+      <c r="E4">
+        <v>0.98039215686274506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -719,12 +744,12 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="n">
-        <v>0.9767441860465116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="n">
+      <c r="E5">
+        <v>0.97674418604651159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -736,12 +761,12 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.972972972972973</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="n">
+      <c r="E6">
+        <v>0.97297297297297303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -753,12 +778,12 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="n">
-        <v>0.9122807017543859</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="n">
+      <c r="E7">
+        <v>0.91228070175438591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -770,12 +795,12 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="n">
-        <v>0.8979591836734694</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="n">
+      <c r="E8">
+        <v>0.89795918367346939</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -787,12 +812,12 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>0.8936170212765957</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -804,12 +829,12 @@
       <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="E10" t="n">
-        <v>0.8846153846153846</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1" t="n">
+      <c r="E10">
+        <v>0.88461538461538458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -821,12 +846,12 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="n">
-        <v>0.8823529411764706</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="n">
+      <c r="E11">
+        <v>0.88235294117647056</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -838,12 +863,12 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="n">
-        <v>0.8695652173913043</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="n">
+      <c r="E12">
+        <v>0.86956521739130432</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -855,12 +880,12 @@
       <c r="D13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>0.8666666666666667</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -872,12 +897,12 @@
       <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>0.8529411764705882</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -889,12 +914,12 @@
       <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="E15" t="n">
-        <v>0.8421052631578947</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1" t="n">
+      <c r="E15">
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -906,12 +931,12 @@
       <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="E16" t="n">
-        <v>0.8387096774193549</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1" t="n">
+      <c r="E16">
+        <v>0.83870967741935487</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -923,12 +948,12 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="E17" t="n">
-        <v>0.835820895522388</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1" t="n">
+      <c r="E17">
+        <v>0.83582089552238803</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -940,12 +965,12 @@
       <c r="D18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="n">
-        <v>0.8260869565217391</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1" t="n">
+      <c r="E18">
+        <v>0.82608695652173914</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -957,12 +982,12 @@
       <c r="D19" t="s">
         <v>32</v>
       </c>
-      <c r="E19" t="n">
-        <v>0.819672131147541</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1" t="n">
+      <c r="E19">
+        <v>0.81967213114754101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -974,12 +999,12 @@
       <c r="D20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" t="n">
-        <v>0.819672131147541</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1" t="n">
+      <c r="E20">
+        <v>0.81967213114754101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -991,12 +1016,12 @@
       <c r="D21" t="s">
         <v>12</v>
       </c>
-      <c r="E21" t="n">
-        <v>0.8181818181818182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1" t="n">
+      <c r="E21">
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -1008,12 +1033,12 @@
       <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="E22" t="n">
-        <v>0.8095238095238095</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1" t="n">
+      <c r="E22">
+        <v>0.80952380952380953</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1025,12 +1050,12 @@
       <c r="D23" t="s">
         <v>36</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>0.8</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -1042,12 +1067,12 @@
       <c r="D24" t="s">
         <v>39</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -1059,12 +1084,12 @@
       <c r="D25" t="s">
         <v>41</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -1076,12 +1101,12 @@
       <c r="D26" t="s">
         <v>14</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>0.8</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="1" t="n">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -1093,12 +1118,12 @@
       <c r="D27" t="s">
         <v>26</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>0.7931034482758621</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="1" t="n">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -1110,12 +1135,12 @@
       <c r="D28" t="s">
         <v>43</v>
       </c>
-      <c r="E28" t="n">
-        <v>0.7924528301886793</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="n">
+      <c r="E28">
+        <v>0.79245283018867929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -1127,12 +1152,12 @@
       <c r="D29" t="s">
         <v>32</v>
       </c>
-      <c r="E29" t="n">
-        <v>0.7887323943661971</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1" t="n">
+      <c r="E29">
+        <v>0.78873239436619713</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -1144,12 +1169,12 @@
       <c r="D30" t="s">
         <v>36</v>
       </c>
-      <c r="E30" t="n">
-        <v>0.7878787878787878</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="1" t="n">
+      <c r="E30">
+        <v>0.78787878787878785</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -1161,12 +1186,12 @@
       <c r="D31" t="s">
         <v>26</v>
       </c>
-      <c r="E31" t="n">
-        <v>0.7837837837837838</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1" t="n">
+      <c r="E31">
+        <v>0.78378378378378377</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -1178,12 +1203,12 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="E32" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1" t="n">
+      <c r="E32">
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
@@ -1195,12 +1220,12 @@
       <c r="D33" t="s">
         <v>10</v>
       </c>
-      <c r="E33" t="n">
-        <v>0.7777777777777778</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="n">
+      <c r="E33">
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
@@ -1212,12 +1237,12 @@
       <c r="D34" t="s">
         <v>48</v>
       </c>
-      <c r="E34" t="n">
-        <v>0.7755102040816326</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1" t="n">
+      <c r="E34">
+        <v>0.77551020408163263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
@@ -1229,12 +1254,12 @@
       <c r="D35" t="s">
         <v>12</v>
       </c>
-      <c r="E35" t="n">
-        <v>0.7741935483870968</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="n">
+      <c r="E35">
+        <v>0.77419354838709675</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
@@ -1246,12 +1271,12 @@
       <c r="D36" t="s">
         <v>50</v>
       </c>
-      <c r="E36" t="n">
-        <v>0.7692307692307693</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="n">
+      <c r="E36">
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
@@ -1263,12 +1288,12 @@
       <c r="D37" t="s">
         <v>13</v>
       </c>
-      <c r="E37" t="n">
-        <v>0.7671232876712328</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="n">
+      <c r="E37">
+        <v>0.76712328767123283</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -1280,12 +1305,12 @@
       <c r="D38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" t="n">
-        <v>0.7659574468085106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1" t="n">
+      <c r="E38">
+        <v>0.76595744680851063</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
@@ -1297,12 +1322,12 @@
       <c r="D39" t="s">
         <v>8</v>
       </c>
-      <c r="E39" t="n">
-        <v>0.7659574468085106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1" t="n">
+      <c r="E39">
+        <v>0.76595744680851063</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
@@ -1314,12 +1339,12 @@
       <c r="D40" t="s">
         <v>53</v>
       </c>
-      <c r="E40" t="n">
-        <v>0.7659574468085106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1" t="n">
+      <c r="E40">
+        <v>0.76595744680851063</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
@@ -1331,12 +1356,12 @@
       <c r="D41" t="s">
         <v>17</v>
       </c>
-      <c r="E41" t="n">
-        <v>0.7647058823529411</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1" t="n">
+      <c r="E41">
+        <v>0.76470588235294112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
@@ -1348,12 +1373,12 @@
       <c r="D42" t="s">
         <v>54</v>
       </c>
-      <c r="E42" t="n">
+      <c r="E42">
         <v>0.759493670886076</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1" t="n">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
@@ -1365,12 +1390,12 @@
       <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="E43" t="n">
-        <v>0.7586206896551724</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1" t="n">
+      <c r="E43">
+        <v>0.75862068965517238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
@@ -1382,12 +1407,12 @@
       <c r="D44" t="s">
         <v>55</v>
       </c>
-      <c r="E44" t="n">
-        <v>0.7540983606557377</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1" t="n">
+      <c r="E44">
+        <v>0.75409836065573765</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
@@ -1399,12 +1424,12 @@
       <c r="D45" t="s">
         <v>57</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E45">
         <v>0.75</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="n">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
@@ -1416,12 +1441,12 @@
       <c r="D46" t="s">
         <v>43</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E46">
         <v>0.75</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1" t="n">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
@@ -1433,12 +1458,12 @@
       <c r="D47" t="s">
         <v>8</v>
       </c>
-      <c r="E47" t="n">
-        <v>0.746268656716418</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1" t="n">
+      <c r="E47">
+        <v>0.74626865671641796</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
@@ -1450,12 +1475,12 @@
       <c r="D48" t="s">
         <v>31</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48">
         <v>0.7441860465116279</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1" t="n">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
@@ -1467,12 +1492,12 @@
       <c r="D49" t="s">
         <v>5</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>0.7441860465116279</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1" t="n">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
@@ -1484,12 +1509,12 @@
       <c r="D50" t="s">
         <v>60</v>
       </c>
-      <c r="E50" t="n">
-        <v>0.7428571428571429</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1" t="n">
+      <c r="E50">
+        <v>0.74285714285714288</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
@@ -1501,12 +1526,12 @@
       <c r="D51" t="s">
         <v>46</v>
       </c>
-      <c r="E51" t="n">
-        <v>0.7368421052631579</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="n">
+      <c r="E51">
+        <v>0.73684210526315785</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
@@ -1518,12 +1543,12 @@
       <c r="D52" t="s">
         <v>21</v>
       </c>
-      <c r="E52" t="n">
-        <v>0.7368421052631579</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1" t="n">
+      <c r="E52">
+        <v>0.73684210526315785</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
@@ -1535,12 +1560,12 @@
       <c r="D53" t="s">
         <v>61</v>
       </c>
-      <c r="E53" t="n">
-        <v>0.7333333333333333</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1" t="n">
+      <c r="E53">
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
@@ -1552,12 +1577,12 @@
       <c r="D54" t="s">
         <v>55</v>
       </c>
-      <c r="E54" t="n">
-        <v>0.7323943661971831</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="1" t="n">
+      <c r="E54">
+        <v>0.73239436619718312</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
@@ -1569,12 +1594,12 @@
       <c r="D55" t="s">
         <v>50</v>
       </c>
-      <c r="E55" t="n">
-        <v>0.7301587301587301</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="1" t="n">
+      <c r="E55">
+        <v>0.73015873015873012</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
@@ -1586,12 +1611,12 @@
       <c r="D56" t="s">
         <v>32</v>
       </c>
-      <c r="E56" t="n">
-        <v>0.7272727272727273</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="1" t="n">
+      <c r="E56">
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
@@ -1603,12 +1628,12 @@
       <c r="D57" t="s">
         <v>14</v>
       </c>
-      <c r="E57" t="n">
-        <v>0.7272727272727273</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="1" t="n">
+      <c r="E57">
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
@@ -1620,12 +1645,12 @@
       <c r="D58" t="s">
         <v>60</v>
       </c>
-      <c r="E58" t="n">
-        <v>0.725</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="1" t="n">
+      <c r="E58">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
@@ -1637,12 +1662,12 @@
       <c r="D59" t="s">
         <v>39</v>
       </c>
-      <c r="E59" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="n">
+      <c r="E59">
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
@@ -1654,12 +1679,12 @@
       <c r="D60" t="s">
         <v>36</v>
       </c>
-      <c r="E60" t="n">
-        <v>0.7222222222222222</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="1" t="n">
+      <c r="E60">
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
@@ -1671,12 +1696,12 @@
       <c r="D61" t="s">
         <v>12</v>
       </c>
-      <c r="E61" t="n">
+      <c r="E61">
         <v>0.72</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="1" t="n">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
@@ -1688,12 +1713,12 @@
       <c r="D62" t="s">
         <v>66</v>
       </c>
-      <c r="E62" t="n">
-        <v>0.717948717948718</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="1" t="n">
+      <c r="E62">
+        <v>0.71794871794871795</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
@@ -1705,12 +1730,12 @@
       <c r="D63" t="s">
         <v>39</v>
       </c>
-      <c r="E63" t="n">
-        <v>0.717948717948718</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="1" t="n">
+      <c r="E63">
+        <v>0.71794871794871795</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
@@ -1722,12 +1747,12 @@
       <c r="D64" t="s">
         <v>61</v>
       </c>
-      <c r="E64" t="n">
-        <v>0.7169811320754716</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="1" t="n">
+      <c r="E64">
+        <v>0.71698113207547165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
@@ -1739,12 +1764,12 @@
       <c r="D65" t="s">
         <v>14</v>
       </c>
-      <c r="E65" t="n">
-        <v>0.7169811320754716</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="1" t="n">
+      <c r="E65">
+        <v>0.71698113207547165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
@@ -1756,12 +1781,12 @@
       <c r="D66" t="s">
         <v>13</v>
       </c>
-      <c r="E66" t="n">
-        <v>0.7169811320754716</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="1" t="n">
+      <c r="E66">
+        <v>0.71698113207547165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
@@ -1773,12 +1798,12 @@
       <c r="D67" t="s">
         <v>69</v>
       </c>
-      <c r="E67" t="n">
-        <v>0.7083333333333334</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="1" t="n">
+      <c r="E67">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
@@ -1790,12 +1815,12 @@
       <c r="D68" t="s">
         <v>71</v>
       </c>
-      <c r="E68" t="n">
-        <v>0.7083333333333334</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="1" t="n">
+      <c r="E68">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
@@ -1807,12 +1832,12 @@
       <c r="D69" t="s">
         <v>73</v>
       </c>
-      <c r="E69" t="n">
-        <v>0.7083333333333334</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="1" t="n">
+      <c r="E69">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
@@ -1824,12 +1849,12 @@
       <c r="D70" t="s">
         <v>15</v>
       </c>
-      <c r="E70" t="n">
-        <v>0.7058823529411765</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="1" t="n">
+      <c r="E70">
+        <v>0.70588235294117652</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
@@ -1841,12 +1866,12 @@
       <c r="D71" t="s">
         <v>54</v>
       </c>
-      <c r="E71" t="n">
-        <v>0.7058823529411765</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="1" t="n">
+      <c r="E71">
+        <v>0.70588235294117652</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
@@ -1858,12 +1883,12 @@
       <c r="D72" t="s">
         <v>28</v>
       </c>
-      <c r="E72" t="n">
-        <v>0.7027027027027027</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="1" t="n">
+      <c r="E72">
+        <v>0.70270270270270274</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
@@ -1875,12 +1900,12 @@
       <c r="D73" t="s">
         <v>55</v>
       </c>
-      <c r="E73" t="n">
-        <v>0.7012987012987013</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="1" t="n">
+      <c r="E73">
+        <v>0.70129870129870131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
@@ -1892,12 +1917,12 @@
       <c r="D74" t="s">
         <v>10</v>
       </c>
-      <c r="E74" t="n">
+      <c r="E74">
         <v>0.7</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="1" t="n">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
@@ -1909,12 +1934,12 @@
       <c r="D75" t="s">
         <v>76</v>
       </c>
-      <c r="E75" t="n">
-        <v>0.6938775510204082</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="1" t="n">
+      <c r="E75">
+        <v>0.69387755102040816</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
@@ -1926,12 +1951,12 @@
       <c r="D76" t="s">
         <v>77</v>
       </c>
-      <c r="E76" t="n">
-        <v>0.6885245901639344</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="1" t="n">
+      <c r="E76">
+        <v>0.68852459016393441</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
@@ -1943,12 +1968,12 @@
       <c r="D77" t="s">
         <v>28</v>
       </c>
-      <c r="E77" t="n">
-        <v>0.6885245901639344</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="1" t="n">
+      <c r="E77">
+        <v>0.68852459016393441</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
@@ -1960,12 +1985,12 @@
       <c r="D78" t="s">
         <v>15</v>
       </c>
-      <c r="E78" t="n">
+      <c r="E78">
         <v>0.6875</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="1" t="n">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
@@ -1977,12 +2002,12 @@
       <c r="D79" t="s">
         <v>43</v>
       </c>
-      <c r="E79" t="n">
-        <v>0.6857142857142857</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="1" t="n">
+      <c r="E79">
+        <v>0.68571428571428572</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
@@ -1994,12 +2019,12 @@
       <c r="D80" t="s">
         <v>79</v>
       </c>
-      <c r="E80" t="n">
-        <v>0.6842105263157895</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="1" t="n">
+      <c r="E80">
+        <v>0.68421052631578949</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
@@ -2011,12 +2036,12 @@
       <c r="D81" t="s">
         <v>41</v>
       </c>
-      <c r="E81" t="n">
-        <v>0.6818181818181818</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="1" t="n">
+      <c r="E81">
+        <v>0.68181818181818177</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
@@ -2028,12 +2053,12 @@
       <c r="D82" t="s">
         <v>21</v>
       </c>
-      <c r="E82" t="n">
+      <c r="E82">
         <v>0.68</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="1" t="n">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
@@ -2045,12 +2070,12 @@
       <c r="D83" t="s">
         <v>82</v>
       </c>
-      <c r="E83" t="n">
+      <c r="E83">
         <v>0.6785714285714286</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="1" t="n">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
@@ -2062,12 +2087,12 @@
       <c r="D84" t="s">
         <v>60</v>
       </c>
-      <c r="E84" t="n">
-        <v>0.6744186046511628</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="1" t="n">
+      <c r="E84">
+        <v>0.67441860465116277</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
@@ -2079,12 +2104,12 @@
       <c r="D85" t="s">
         <v>54</v>
       </c>
-      <c r="E85" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="1" t="n">
+      <c r="E85">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
@@ -2096,12 +2121,12 @@
       <c r="D86" t="s">
         <v>73</v>
       </c>
-      <c r="E86" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="1" t="n">
+      <c r="E86">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
@@ -2113,12 +2138,12 @@
       <c r="D87" t="s">
         <v>61</v>
       </c>
-      <c r="E87" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="1" t="n">
+      <c r="E87">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
@@ -2130,12 +2155,12 @@
       <c r="D88" t="s">
         <v>31</v>
       </c>
-      <c r="E88" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="1" t="n">
+      <c r="E88">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
@@ -2147,12 +2172,12 @@
       <c r="D89" t="s">
         <v>21</v>
       </c>
-      <c r="E89" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" s="1" t="n">
+      <c r="E89">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
@@ -2164,12 +2189,12 @@
       <c r="D90" t="s">
         <v>50</v>
       </c>
-      <c r="E90" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" s="1" t="n">
+      <c r="E90">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
@@ -2181,12 +2206,12 @@
       <c r="D91" t="s">
         <v>84</v>
       </c>
-      <c r="E91" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" s="1" t="n">
+      <c r="E91">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
@@ -2198,12 +2223,12 @@
       <c r="D92" t="s">
         <v>14</v>
       </c>
-      <c r="E92" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" s="1" t="n">
+      <c r="E92">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
@@ -2215,12 +2240,12 @@
       <c r="D93" t="s">
         <v>36</v>
       </c>
-      <c r="E93" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="1" t="n">
+      <c r="E93">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
@@ -2232,12 +2257,12 @@
       <c r="D94" t="s">
         <v>46</v>
       </c>
-      <c r="E94" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="1" t="n">
+      <c r="E94">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
@@ -2249,12 +2274,12 @@
       <c r="D95" t="s">
         <v>46</v>
       </c>
-      <c r="E95" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="A96" s="1" t="n">
+      <c r="E95">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
@@ -2266,12 +2291,12 @@
       <c r="D96" t="s">
         <v>88</v>
       </c>
-      <c r="E96" t="n">
-        <v>0.6666666666666666</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="1" t="n">
+      <c r="E96">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
@@ -2283,12 +2308,12 @@
       <c r="D97" t="s">
         <v>13</v>
       </c>
-      <c r="E97" t="n">
+      <c r="E97">
         <v>0.65625</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="1" t="n">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
@@ -2300,12 +2325,12 @@
       <c r="D98" t="s">
         <v>79</v>
       </c>
-      <c r="E98" t="n">
-        <v>0.6551724137931034</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="1" t="n">
+      <c r="E98">
+        <v>0.65517241379310343</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" t="s">
@@ -2317,11 +2342,11 @@
       <c r="D99" t="s">
         <v>5</v>
       </c>
-      <c r="E99" t="n">
-        <v>0.6530612244897959</v>
+      <c r="E99">
+        <v>0.65306122448979587</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>